<commit_message>
added class 1 activities
</commit_message>
<xml_diff>
--- a/lesson-1/1-Student-Resources/02-Stu_GradeBook/Unsolved/GradeBook_Unsolved.xlsx
+++ b/lesson-1/1-Student-Resources/02-Stu_GradeBook/Unsolved/GradeBook_Unsolved.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\1\Activities\08-Stu_GradeBook\Unsolved\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertovaldez/tec-data/lesson-1/1-Student-Resources/02-Stu_GradeBook/Unsolved/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F38F79-CEDD-9248-954C-077A77588286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12780"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -125,8 +136,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +149,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,7 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -181,6 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -495,21 +515,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="10" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -553,7 +579,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -571,7 +597,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -589,7 +615,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -607,7 +633,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -625,7 +651,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -643,7 +669,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -661,7 +687,7 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -679,7 +705,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -697,7 +723,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -715,7 +741,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -733,7 +759,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -751,7 +777,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -769,7 +795,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -787,7 +813,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -805,7 +831,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -823,7 +849,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -841,7 +867,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -859,7 +885,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -877,7 +903,7 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -895,7 +921,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -913,7 +939,7 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -931,7 +957,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -949,7 +975,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -966,6 +992,14 @@
         <v>53</v>
       </c>
       <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="H26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>